<commit_message>
integrated gui and api test
</commit_message>
<xml_diff>
--- a/Search Reservation/Default.xlsx
+++ b/Search Reservation/Default.xlsx
@@ -12,6 +12,14 @@
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+  <si>
+    <t>arg_ReservationNumber</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,10 +481,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.2578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row customFormat="1">
+      <c t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>